<commit_message>
simplified the revision lab for lever 3
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA\0-C# New\Slides and labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74951163-D4C9-409D-AF19-B5E11EB86A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A47E01D-769D-472B-8D82-56F76812AE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{52FCE2D1-3CD9-4802-852E-8BD5EFB04241}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>Introductopn</t>
   </si>
@@ -139,10 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7F6BA2-4695-4149-A832-BB73A46B745F}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,29 +796,40 @@
         <v>4.583333333333333</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -828,7 +840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -839,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -847,15 +859,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39">
-        <f>SUM(B34:B38)</f>
-        <v>270</v>
-      </c>
-      <c r="C39" s="1">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3">
+        <f>SUM(B33:B38)</f>
+        <v>290</v>
+      </c>
+      <c r="C39" s="2">
         <f>B39/60</f>
-        <v>4.5</v>
-      </c>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enhanced slides 2 and 3
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA\0-C# New\Slides and labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A47E01D-769D-472B-8D82-56F76812AE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BA5B83-8B37-426F-BA9D-345E8879D280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{52FCE2D1-3CD9-4802-852E-8BD5EFB04241}"/>
+    <workbookView xWindow="-36870" yWindow="1530" windowWidth="17280" windowHeight="15525" xr2:uid="{52FCE2D1-3CD9-4802-852E-8BD5EFB04241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>Introductopn</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Day = 6 hours</t>
+  </si>
+  <si>
+    <t>Done in day 1</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +569,9 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">

</xml_diff>